<commit_message>
2024-09-13 @ 09:55 - v4.I.1.xlsb
- LastRow ---> lastRow
- Améliorations à chk_TEC
- Ajustements à TEC_Analyse
- Ajustements (affichage) à Fn_Complete_Date
- Ajustements (log) à TEC_Saisie
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CA72DFC-8181-4FC7-9EED-15731E3A026B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D8809D-2D4F-47B5-8C8B-6846FB3EA6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{72DD8F7C-5491-479C-928E-7CAE306232B3}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$2:$F$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$2:$F$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,9 +44,6 @@
     <t>Brouillon : Ôter la protection sur la section « Charges pour le client » pour me permettre d’accéder à voir tout le contenu des cellules qui est plus long que la cellule. Idem pour la section « Sommaire des heures et des taux selon la requête de facturation » pour me permettre d’y rentrer les heures et taux souhaitées ;</t>
   </si>
   <si>
-    <t>Brouillon : Pour la validation de données, t’assurer que dans Alertes d’erreur, la case « Quand des donn.es sont tapées » est décochée ;</t>
-  </si>
-  <si>
     <t>Brouillon : prévoir que la date par défaut est la date de la journée que je prépare la facture ;</t>
   </si>
   <si>
@@ -147,13 +144,16 @@
   </si>
   <si>
     <t>Ajouter la possibilité d’envoyer un rappel au bout de 30 jours pour tous les comptes non reçu que je peux désélectionner si je ne veux pas leurs envoyer de rappel. Par la suite, une fois le 30 jours passé, prévoir des rappels aux 2 semaines et après 60 jours des rappels à chaque semaine.</t>
+  </si>
+  <si>
+    <t>Brouillon : Pour la validation de données, t’assurer que dans Alertes d’erreur, la case « Quand des données sont tapées » est décochée ;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +196,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="16"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -223,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -250,6 +282,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -586,13 +630,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBAF87A-5A44-4B5F-8603-257FAFA1F2A1}">
-  <sheetPr>
+  <sheetPr codeName="Feuil1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,146 +651,146 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>23</v>
@@ -755,49 +799,49 @@
         <v>7</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>23</v>
@@ -806,24 +850,24 @@
         <v>10</v>
       </c>
       <c r="E12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>29</v>
@@ -831,136 +875,138 @@
     </row>
     <row r="14" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="E18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="8" t="s">
+    </row>
+    <row r="20" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="13" t="s">
         <v>28</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B20" xr:uid="{4ED43C6F-40AA-4AD7-AE34-E9349EC73289}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B16 B17:B20" xr:uid="{4ED43C6F-40AA-4AD7-AE34-E9349EC73289}">
       <formula1>"0_Bogue fonctionnel,1_Bogue agaçant,2_Amélioration,3_Performance"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C20" xr:uid="{7BE2BF95-B0BB-4944-BF2F-C483CFA6532A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C16 C17:C20" xr:uid="{7BE2BF95-B0BB-4944-BF2F-C483CFA6532A}">
       <formula1>"0_ASAP,1_Semaine,2_Futur"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E20" xr:uid="{1C2EE06E-B0A4-4E3D-95EA-0EB59086432A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E16 E17:E20" xr:uid="{1C2EE06E-B0A4-4E3D-95EA-0EB59086432A}">
       <formula1>"A,B,C"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F20" xr:uid="{7484232B-0EEF-4351-A081-06D5B4AEBF2D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F16 F17:F20" xr:uid="{7484232B-0EEF-4351-A081-06D5B4AEBF2D}">
       <formula1>"1 Heure,2 à 3 heures,4 @ 7 heures,Plus de 8 heures"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
2024_09_24 @ 13:44  - Clients_v2.4.xlsm
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D8809D-2D4F-47B5-8C8B-6846FB3EA6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61230C6-BC34-4775-8540-DA55379F9893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{72DD8F7C-5491-479C-928E-7CAE306232B3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{72DD8F7C-5491-479C-928E-7CAE306232B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$2:$F$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$2:$F$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="44">
   <si>
     <t>Brouillon : Ôter la protection sur la section « Charges pour le client » pour me permettre d’accéder à voir tout le contenu des cellules qui est plus long que la cellule. Idem pour la section « Sommaire des heures et des taux selon la requête de facturation » pour me permettre d’y rentrer les heures et taux souhaitées ;</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Dans Confirmation de Facture : Après avoir confirmé une facture, nous amener tout de suite sur la facture suivante à approuver et ajouter une possibilité d’approuver toutes les factures d’un seul coup ;</t>
   </si>
   <si>
-    <t>Dans Fac_finale la police n’est pas toute 98-88-80, svp modifier ;</t>
-  </si>
-  <si>
     <t>Comment est-ce possible de mettre du temps comme facturé sans faire de facture : ex : Patrick et Jean Lessard – j’ai été payé comptant je ne ferai pas de facture et je veux supprimer leur temps des Travaux en cours à facturer. Autre exemple : Le temps de Vladimir dans Clinique d’optométrie Lachenaie aurait dû aller dans Dr Frédéric Morin que j’ai déjà facturer et je ne pourrai pas refacturer le client pour cette portion que je n’avais pas vue. Autre exemple : 9389-8179 – Daniel O’Reilley – échange de services donc je ne veux pas le lui facturer le temps au dossier. Éric Berthiaume que je ne facturerai jamais car prospection que je n’aurai pas ;</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>Parfois, la fonction demande de facture ne fonctionne pas même en pesant dans la colonne C ou H : le temps à charger et la case à facturer n’apparait pas ;</t>
   </si>
   <si>
-    <t xml:space="preserve">Dans Demande de factures, idéalement on ne veut pas voir les dossiers non facturables x-Administratif … </t>
-  </si>
-  <si>
     <t>Quand je suis dans Brouillon, dans la recherche de client, si je tape « édition » il ne trouve pas de client mais si je tape « Édition » il va trouver … juste la majuscule, il faudrait pouvoir trouver avec ou sans la majuscule ;</t>
   </si>
   <si>
@@ -86,9 +80,6 @@
     <t>Dans Facture Finale, lorsque je pèse sur Création du PDF, il crée le PDF et me demande dans quel fichier Excel ajouter l’onglet de la facture. Dans le cas des nouveaux clients, il n’y a pas de fichier Excel, est-ce possible de prévoir quelque chose pour les nouveaux clients qui n’ont pas de fichiers Excel?</t>
   </si>
   <si>
-    <t>Dans la Liste âgée des comptes clients, est-ce possible de ne pas montrer les clients à 0$ mais de laisser une case qui me permettrait au besoin de voir ceux qui sont à 0$ svp? Pour ceux qui sont encaissés, est-ce possible d’indiquer la date de perception dans une autre colonne?</t>
-  </si>
-  <si>
     <t>2024-09-07-Courriel_GC</t>
   </si>
   <si>
@@ -146,14 +137,107 @@
     <t>Ajouter la possibilité d’envoyer un rappel au bout de 30 jours pour tous les comptes non reçu que je peux désélectionner si je ne veux pas leurs envoyer de rappel. Par la suite, une fois le 30 jours passé, prévoir des rappels aux 2 semaines et après 60 jours des rappels à chaque semaine.</t>
   </si>
   <si>
-    <t>Brouillon : Pour la validation de données, t’assurer que dans Alertes d’erreur, la case « Quand des données sont tapées » est décochée ;</t>
+    <t>2024-09-23-Courriel_GC</t>
+  </si>
+  <si>
+    <t>2024-09-24-Courriel_GC</t>
+  </si>
+  <si>
+    <t>Impossible de détruire un CLIENT même s'il n'a pas de transactions dans le Système… Exemple client '118'</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>2024-09-23-Courriel_ML</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Si une charge est à l'écran pour modifier, ET qu'il n'y a rien à modifier, il n'y a pas de façon de continuer
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Corrigé avec  Version 4.I.3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dans Fac_finale la police n’est pas toute 98-88-80, svp modifier
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Corrigé avec  Version 4.I.3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dans la Liste âgée des comptes clients, est-ce possible de ne pas montrer les clients à 0$ mais de laisser une case qui me permettrait au besoin de voir ceux qui sont à 0$ svp? Pour ceux qui sont encaissés, est-ce possible d’indiquer la date de perception dans une autre colonne?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Corrigé avec Version 4.I.2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Brouillon : Pour la validation de données, t’assurer que dans Alertes d’erreur, la case « Quand des données sont tapées » est décochée ;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Corrigé avec Version 4.I.3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dans Demande de factures, idéalement on ne veut pas voir les dossiers non facturables x-Administratif …
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Corrigé avec Version 4.I.3</t>
+    </r>
+  </si>
+  <si>
+    <t>Accès à des statistiques d'heures à partir de la Saisie des Heures (long courriel explicatif de la part de Michel)</t>
+  </si>
+  <si>
+    <t>La touche NUM LOCK s'active / se désactive, dans la saisie des Heures</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,37 +283,47 @@
     <font>
       <strike/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <strike/>
       <sz val="16"/>
-      <color rgb="FF0070C0"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <strike/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +333,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -255,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -284,16 +384,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -633,255 +734,255 @@
   <sheetPr codeName="Feuil1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="100.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="100.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="E8" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F9" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E11" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>27</v>
@@ -890,128 +991,205 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>28</v>
+      <c r="F19" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="10" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F20">
+    <sortCondition ref="A2:A20"/>
+    <sortCondition ref="E2:E20"/>
+    <sortCondition ref="F2:F20"/>
+    <sortCondition ref="B2:B20"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B16 B17:B20" xr:uid="{4ED43C6F-40AA-4AD7-AE34-E9349EC73289}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3:B24" xr:uid="{4ED43C6F-40AA-4AD7-AE34-E9349EC73289}">
       <formula1>"0_Bogue fonctionnel,1_Bogue agaçant,2_Amélioration,3_Performance"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C16 C17:C20" xr:uid="{7BE2BF95-B0BB-4944-BF2F-C483CFA6532A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C3:C24" xr:uid="{7BE2BF95-B0BB-4944-BF2F-C483CFA6532A}">
       <formula1>"0_ASAP,1_Semaine,2_Futur"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E16 E17:E20" xr:uid="{1C2EE06E-B0A4-4E3D-95EA-0EB59086432A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2 E3:E24" xr:uid="{1C2EE06E-B0A4-4E3D-95EA-0EB59086432A}">
       <formula1>"A,B,C"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F16 F17:F20" xr:uid="{7484232B-0EEF-4351-A081-06D5B4AEBF2D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F3:F24" xr:uid="{7484232B-0EEF-4351-A081-06D5B4AEBF2D}">
       <formula1>"1 Heure,2 à 3 heures,4 @ 7 heures,Plus de 8 heures"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.6692913385826772" bottom="0.59055118110236227" header="0.11811023622047245" footer="0.11811023622047245"/>
-  <pageSetup scale="78" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="77" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;9
 &amp;D - &amp;T&amp;C&amp;9

</xml_diff>

<commit_message>
2024-09-24 @ 15:02 -APP_v4.I.3.xlsb
- Intégration de la logique des clients NON-FACTURABLES & révision des calculs (TDB, Analyse des TEC, Vérification d'intégrité, etc.)
- Ajout d'une colonne dans TEC_TDB_Data (CodeClient)
- Nouvelle fonction (Fn_Is_Client_Facturable)
- Exclusion des clients NON-FACTURABLES du traitement de l'analyse des TEC
- Tests sur le démarrage de l'application
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61230C6-BC34-4775-8540-DA55379F9893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906FCA0C-D782-4135-887D-FA1896E174B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{72DD8F7C-5491-479C-928E-7CAE306232B3}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$2:$F$24</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Feuil1!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$2:$F$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="51">
   <si>
     <t>Brouillon : Ôter la protection sur la section « Charges pour le client » pour me permettre d’accéder à voir tout le contenu des cellules qui est plus long que la cellule. Idem pour la section « Sommaire des heures et des taux selon la requête de facturation » pour me permettre d’y rentrer les heures et taux souhaitées ;</t>
   </si>
@@ -80,9 +81,6 @@
     <t>Dans Facture Finale, lorsque je pèse sur Création du PDF, il crée le PDF et me demande dans quel fichier Excel ajouter l’onglet de la facture. Dans le cas des nouveaux clients, il n’y a pas de fichier Excel, est-ce possible de prévoir quelque chose pour les nouveaux clients qui n’ont pas de fichiers Excel?</t>
   </si>
   <si>
-    <t>2024-09-07-Courriel_GC</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -137,19 +135,10 @@
     <t>Ajouter la possibilité d’envoyer un rappel au bout de 30 jours pour tous les comptes non reçu que je peux désélectionner si je ne veux pas leurs envoyer de rappel. Par la suite, une fois le 30 jours passé, prévoir des rappels aux 2 semaines et après 60 jours des rappels à chaque semaine.</t>
   </si>
   <si>
-    <t>2024-09-23-Courriel_GC</t>
-  </si>
-  <si>
-    <t>2024-09-24-Courriel_GC</t>
-  </si>
-  <si>
     <t>Impossible de détruire un CLIENT même s'il n'a pas de transactions dans le Système… Exemple client '118'</t>
   </si>
   <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>2024-09-23-Courriel_ML</t>
   </si>
   <si>
     <r>
@@ -232,12 +221,45 @@
   <si>
     <t>La touche NUM LOCK s'active / se désactive, dans la saisie des Heures</t>
   </si>
+  <si>
+    <t>2024-09-24-RMV</t>
+  </si>
+  <si>
+    <t>Finaliser les transactions pour le mois d'août</t>
+  </si>
+  <si>
+    <t>2024-09-07-GC_Courriel</t>
+  </si>
+  <si>
+    <t>2024-09-23-GC_Courriel</t>
+  </si>
+  <si>
+    <t>2024-09-24-GC_Courriel</t>
+  </si>
+  <si>
+    <t>2024-09-23-ML_Courriel</t>
+  </si>
+  <si>
+    <t>Les premières insctructions de code ne sont pas enregistrées dans le log…</t>
+  </si>
+  <si>
+    <t>Les sauvegardes ne sont pont plus pour le fichier MASTER.xlsx</t>
+  </si>
+  <si>
+    <t>2024-09-06-RMV</t>
+  </si>
+  <si>
+    <t>Problème avec le format de date pour les 12 premiers jours du mois…</t>
+  </si>
+  <si>
+    <t>2024-09-20-RMV</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +344,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -343,7 +373,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -351,18 +381,147 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -372,30 +531,80 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -734,457 +943,549 @@
   <sheetPr codeName="Feuil1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="100.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" style="6" customWidth="1"/>
+    <col min="1" max="1" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="100.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="D11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="D17" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="D18" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
+      <c r="B24" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="25" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="D25" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    </row>
+    <row r="26" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="D26" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
+    </row>
+    <row r="27" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="19"/>
+      <c r="B27" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="D28" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="10" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>25</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F20">
-    <sortCondition ref="A2:A20"/>
-    <sortCondition ref="E2:E20"/>
-    <sortCondition ref="F2:F20"/>
-    <sortCondition ref="B2:B20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F23">
+    <sortCondition ref="A2:A23"/>
+    <sortCondition ref="B2:B23"/>
+    <sortCondition ref="E2:E23"/>
+    <sortCondition ref="F2:F23"/>
+    <sortCondition ref="C2:C23"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3:B24" xr:uid="{4ED43C6F-40AA-4AD7-AE34-E9349EC73289}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C3:C22 C23:C28" xr:uid="{4ED43C6F-40AA-4AD7-AE34-E9349EC73289}">
       <formula1>"0_Bogue fonctionnel,1_Bogue agaçant,2_Amélioration,3_Performance"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C3:C24" xr:uid="{7BE2BF95-B0BB-4944-BF2F-C483CFA6532A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2 A3:A22 A23:A28" xr:uid="{7BE2BF95-B0BB-4944-BF2F-C483CFA6532A}">
       <formula1>"0_ASAP,1_Semaine,2_Futur"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2 E3:E24" xr:uid="{1C2EE06E-B0A4-4E3D-95EA-0EB59086432A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2 E3:E22 E23:E28" xr:uid="{1C2EE06E-B0A4-4E3D-95EA-0EB59086432A}">
       <formula1>"A,B,C"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F3:F24" xr:uid="{7484232B-0EEF-4351-A081-06D5B4AEBF2D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F3:F22 F23:F28" xr:uid="{7484232B-0EEF-4351-A081-06D5B4AEBF2D}">
       <formula1>"1 Heure,2 à 3 heures,4 @ 7 heures,Plus de 8 heures"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
2024-09-25 @ 06:16 - Clients_v2.6 xlsm
- modUtils - Éliminer un Debug.print, exclure le fichier 'Vérification de la liste de clients.xlsx' de la vérification
- ufClientsMF.frm - Tests & ajustements sur la destruction d'un client
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906FCA0C-D782-4135-887D-FA1896E174B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E88F88C-40D1-4876-8F98-A59CF9E7479F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{72DD8F7C-5491-479C-928E-7CAE306232B3}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Feuil1!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$2:$F$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$2:$F$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="51">
   <si>
     <t>Brouillon : Ôter la protection sur la section « Charges pour le client » pour me permettre d’accéder à voir tout le contenu des cellules qui est plus long que la cellule. Idem pour la section « Sommaire des heures et des taux selon la requête de facturation » pour me permettre d’y rentrer les heures et taux souhaitées ;</t>
   </si>
@@ -135,10 +135,72 @@
     <t>Ajouter la possibilité d’envoyer un rappel au bout de 30 jours pour tous les comptes non reçu que je peux désélectionner si je ne veux pas leurs envoyer de rappel. Par la suite, une fois le 30 jours passé, prévoir des rappels aux 2 semaines et après 60 jours des rappels à chaque semaine.</t>
   </si>
   <si>
-    <t>Impossible de détruire un CLIENT même s'il n'a pas de transactions dans le Système… Exemple client '118'</t>
-  </si>
-  <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Accès à des statistiques d'heures à partir de la Saisie des Heures (long courriel explicatif de la part de Michel)</t>
+  </si>
+  <si>
+    <t>La touche NUM LOCK s'active / se désactive, dans la saisie des Heures</t>
+  </si>
+  <si>
+    <t>Finaliser les transactions pour le mois d'août</t>
+  </si>
+  <si>
+    <t>2024-09-07-GC_Courriel</t>
+  </si>
+  <si>
+    <t>2024-09-23-GC_Courriel</t>
+  </si>
+  <si>
+    <t>2024-09-24-GC_Courriel</t>
+  </si>
+  <si>
+    <t>2024-09-23-ML_Courriel</t>
+  </si>
+  <si>
+    <t>Les sauvegardes ne sont pont plus pour le fichier MASTER.xlsx</t>
+  </si>
+  <si>
+    <t>2024-09-06-RMV</t>
+  </si>
+  <si>
+    <t>Problème avec le format de date pour les 12 premiers jours du mois…</t>
+  </si>
+  <si>
+    <t>2024-09-20-RMV</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Impossible de détruire un CLIENT même s'il n'a pas de transactions dans le Système… Exemple client '118'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Corrigé avec Version Clients_v2.5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Les premières insctructions de code ne sont pas enregistrées dans le log
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Corrigé avec Version 4.I.5</t>
+    </r>
   </si>
   <si>
     <r>
@@ -147,6 +209,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
@@ -157,11 +220,44 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Dans Demande de factures, idéalement on ne veut pas voir les dossiers non facturables x-Administratif …
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Corrigé avec Version 4.I.3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Brouillon : Pour la validation de données, t’assurer que dans Alertes d’erreur, la case « Quand des données sont tapées » est décochée ;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Corrigé avec Version 4.I.3</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Dans Fac_finale la police n’est pas toute 98-88-80, svp modifier
 </t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
@@ -177,6 +273,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
@@ -186,73 +283,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Brouillon : Pour la validation de données, t’assurer que dans Alertes d’erreur, la case « Quand des données sont tapées » est décochée ;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Corrigé avec Version 4.I.3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dans Demande de factures, idéalement on ne veut pas voir les dossiers non facturables x-Administratif …
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Corrigé avec Version 4.I.3</t>
-    </r>
-  </si>
-  <si>
-    <t>Accès à des statistiques d'heures à partir de la Saisie des Heures (long courriel explicatif de la part de Michel)</t>
-  </si>
-  <si>
-    <t>La touche NUM LOCK s'active / se désactive, dans la saisie des Heures</t>
-  </si>
-  <si>
-    <t>2024-09-24-RMV</t>
-  </si>
-  <si>
-    <t>Finaliser les transactions pour le mois d'août</t>
-  </si>
-  <si>
-    <t>2024-09-07-GC_Courriel</t>
-  </si>
-  <si>
-    <t>2024-09-23-GC_Courriel</t>
-  </si>
-  <si>
-    <t>2024-09-24-GC_Courriel</t>
-  </si>
-  <si>
-    <t>2024-09-23-ML_Courriel</t>
-  </si>
-  <si>
-    <t>Les premières insctructions de code ne sont pas enregistrées dans le log…</t>
-  </si>
-  <si>
-    <t>Les sauvegardes ne sont pont plus pour le fichier MASTER.xlsx</t>
-  </si>
-  <si>
-    <t>2024-09-06-RMV</t>
-  </si>
-  <si>
-    <t>Problème avec le format de date pour les 12 premiers jours du mois…</t>
-  </si>
-  <si>
-    <t>2024-09-20-RMV</t>
+    <t>Tableau de bord pour les heures - Semaine, mois &amp; année - Sliders</t>
   </si>
 </sst>
 </file>
@@ -312,12 +343,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -352,6 +377,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -546,7 +578,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -561,7 +593,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -576,34 +608,34 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -943,10 +975,10 @@
   <sheetPr codeName="Feuil1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,31 +1015,31 @@
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="10" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>23</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="15" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>23</v>
@@ -1016,34 +1048,34 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>23</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>23</v>
@@ -1055,13 +1087,13 @@
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>23</v>
@@ -1070,16 +1102,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>23</v>
@@ -1091,13 +1123,13 @@
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>23</v>
@@ -1106,34 +1138,34 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>23</v>
@@ -1142,16 +1174,16 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>23</v>
@@ -1160,34 +1192,34 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>23</v>
@@ -1196,34 +1228,34 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>26</v>
@@ -1232,52 +1264,52 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>26</v>
@@ -1286,37 +1318,37 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="15" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>39</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F20" s="18" t="s">
         <v>25</v>
@@ -1325,67 +1357,67 @@
     <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E21" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="20" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="E24" s="22" t="s">
         <v>23</v>
@@ -1394,16 +1426,16 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="20" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E25" s="22" t="s">
         <v>23</v>
@@ -1412,16 +1444,16 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="20" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E26" s="22" t="s">
         <v>23</v>
@@ -1430,62 +1462,80 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="20" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F27" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="25" t="s">
+      <c r="A28" s="19"/>
+      <c r="B28" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="E28" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="28" t="s">
-        <v>24</v>
+      <c r="D29" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F23">
-    <sortCondition ref="A2:A23"/>
-    <sortCondition ref="B2:B23"/>
-    <sortCondition ref="E2:E23"/>
-    <sortCondition ref="F2:F23"/>
-    <sortCondition ref="C2:C23"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
+    <sortCondition ref="A2:A22"/>
+    <sortCondition ref="B2:B22"/>
+    <sortCondition ref="E2:E22"/>
+    <sortCondition ref="F2:F22"/>
+    <sortCondition ref="C2:C22"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C3:C22 C23:C28" xr:uid="{4ED43C6F-40AA-4AD7-AE34-E9349EC73289}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C29" xr:uid="{4ED43C6F-40AA-4AD7-AE34-E9349EC73289}">
       <formula1>"0_Bogue fonctionnel,1_Bogue agaçant,2_Amélioration,3_Performance"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2 A3:A22 A23:A28" xr:uid="{7BE2BF95-B0BB-4944-BF2F-C483CFA6532A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A29" xr:uid="{7BE2BF95-B0BB-4944-BF2F-C483CFA6532A}">
       <formula1>"0_ASAP,1_Semaine,2_Futur"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2 E3:E22 E23:E28" xr:uid="{1C2EE06E-B0A4-4E3D-95EA-0EB59086432A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E29" xr:uid="{1C2EE06E-B0A4-4E3D-95EA-0EB59086432A}">
       <formula1>"A,B,C"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F3:F22 F23:F28" xr:uid="{7484232B-0EEF-4351-A081-06D5B4AEBF2D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F29" xr:uid="{7484232B-0EEF-4351-A081-06D5B4AEBF2D}">
       <formula1>"1 Heure,2 à 3 heures,4 @ 7 heures,Plus de 8 heures"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>